<commit_message>
read_ts_xlsx and read_ts_csv can now read files with periods but without variables correctly.
</commit_message>
<xml_diff>
--- a/pkg/tests/testthat/read_ts/xlsx/weird_3.xlsx
+++ b/pkg/tests/testthat/read_ts/xlsx/weird_3.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -125,19 +125,19 @@
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="X24" activeCellId="0" sqref="X24"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="5" min="2" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50510204081633"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="2" style="0" width="12.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.51"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -167,7 +167,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>